<commit_message>
Finalizou Dicionário de dados, atualizou as cardinalidades, gerou novo modelo lógico
</commit_message>
<xml_diff>
--- a/db/Dicionário_dados.xlsx
+++ b/db/Dicionário_dados.xlsx
@@ -8,24 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\4DSN_val\BD_conceitual_repairIQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DE34B0-D31B-443F-9451-05D6F8AF201F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D65CA2-6DBB-4EE7-9BFA-2145262DB27A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relacionamento" sheetId="4" r:id="rId1"/>
-    <sheet name="ATRIBUTOS" sheetId="1" r:id="rId2"/>
-    <sheet name="ATRIBUTOS (2)" sheetId="13" r:id="rId3"/>
-    <sheet name="ATRIBUTOS (3)" sheetId="14" r:id="rId4"/>
-    <sheet name="ATRIBUTOS (4)" sheetId="15" r:id="rId5"/>
-    <sheet name="ATRIBUTOS (5)" sheetId="16" r:id="rId6"/>
+    <sheet name="EQUIPAMENTO" sheetId="1" r:id="rId2"/>
+    <sheet name="ORDEM DE SEV." sheetId="13" r:id="rId3"/>
+    <sheet name="OCORRENCIA" sheetId="14" r:id="rId4"/>
+    <sheet name="FUNCIONARIO" sheetId="15" r:id="rId5"/>
+    <sheet name="GRUPO FUNCIONARIO" sheetId="16" r:id="rId6"/>
+    <sheet name="NOTIFICACAO" sheetId="18" r:id="rId7"/>
+    <sheet name="REGISTRO AUDITORIA" sheetId="19" r:id="rId8"/>
+    <sheet name="PREDITIVA IA" sheetId="20" r:id="rId9"/>
+    <sheet name="MODELO ORDEM SERVICO" sheetId="21" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
   <si>
     <t>Relacionamento</t>
   </si>
@@ -124,6 +128,336 @@
   </si>
   <si>
     <t>modela</t>
+  </si>
+  <si>
+    <t>Gera manutenção</t>
+  </si>
+  <si>
+    <t>É gerada algum tipo de manutenção</t>
+  </si>
+  <si>
+    <t>Executa as manutenções, conforme são passadas</t>
+  </si>
+  <si>
+    <t>Recebe notificações sobre manutenção</t>
+  </si>
+  <si>
+    <t>É a formalização sobre o tipo de manutenção</t>
+  </si>
+  <si>
+    <t>É feita sobre as atividades realizadas</t>
+  </si>
+  <si>
+    <t>É realizada para gerar a CBM e TBM</t>
+  </si>
+  <si>
+    <t>Gera o tipo de ordem de serviço</t>
+  </si>
+  <si>
+    <t>Direciona para atividade diaria</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>numero_serie</t>
+  </si>
+  <si>
+    <t>localizacao</t>
+  </si>
+  <si>
+    <t>data_aquisicao</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>5 bytes</t>
+  </si>
+  <si>
+    <t>40 bytes</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>30 bytes</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>10 bytes</t>
+  </si>
+  <si>
+    <t>2 bytes</t>
+  </si>
+  <si>
+    <t>PK not null</t>
+  </si>
+  <si>
+    <t>not null</t>
+  </si>
+  <si>
+    <t>nome do equipamento</t>
+  </si>
+  <si>
+    <t>tipo do equipamento</t>
+  </si>
+  <si>
+    <t>numero_serie do equipamento</t>
+  </si>
+  <si>
+    <t>localizacao do equipamento</t>
+  </si>
+  <si>
+    <t>data_aquisicao do equipamento</t>
+  </si>
+  <si>
+    <t>status do equipamento</t>
+  </si>
+  <si>
+    <t>data_abertura</t>
+  </si>
+  <si>
+    <t>data_fechamento</t>
+  </si>
+  <si>
+    <t>prioridade</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>20 bytes</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 147 bytes</t>
+  </si>
+  <si>
+    <t>5 byte</t>
+  </si>
+  <si>
+    <t>FK not null</t>
+  </si>
+  <si>
+    <t>data_abertura da ordem de serviço</t>
+  </si>
+  <si>
+    <t>data_fechamento da ordem de serviço</t>
+  </si>
+  <si>
+    <t>prioridade da ordem de serviço</t>
+  </si>
+  <si>
+    <t>status da ordem de serviço</t>
+  </si>
+  <si>
+    <t>descricao da ordem de serviço</t>
+  </si>
+  <si>
+    <t>data_ocorrencia</t>
+  </si>
+  <si>
+    <t>status da ocorrencia</t>
+  </si>
+  <si>
+    <t>descrição da ocorrencia</t>
+  </si>
+  <si>
+    <t>data da ocorrencia</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 37 bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nome </t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>64 bytes</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>nome do funcionario</t>
+  </si>
+  <si>
+    <t>login do funcionario</t>
+  </si>
+  <si>
+    <t>senha do funcionario</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 129 bytes</t>
+  </si>
+  <si>
+    <t>nome_grupo</t>
+  </si>
+  <si>
+    <t>descricoes</t>
+  </si>
+  <si>
+    <t>permicoes</t>
+  </si>
+  <si>
+    <t>4 bytes</t>
+  </si>
+  <si>
+    <t>chave primaria com auto incremento</t>
+  </si>
+  <si>
+    <t>chave estrangeira ocorrencia da ordem de serviço</t>
+  </si>
+  <si>
+    <t>chave estrangeira modelo ordem servico da ordem de serviço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nome do grupo </t>
+  </si>
+  <si>
+    <t>descriçoes do grupo</t>
+  </si>
+  <si>
+    <t>permiçoes do grupo</t>
+  </si>
+  <si>
+    <t>data_envio</t>
+  </si>
+  <si>
+    <t>mensagem</t>
+  </si>
+  <si>
+    <t>lida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data de envio </t>
+  </si>
+  <si>
+    <t>mensagem de notificação</t>
+  </si>
+  <si>
+    <t>se foi lida ao ser entregue</t>
+  </si>
+  <si>
+    <t>tipo de O.S</t>
+  </si>
+  <si>
+    <t>60 bytes</t>
+  </si>
+  <si>
+    <t>acao</t>
+  </si>
+  <si>
+    <t>data_acao</t>
+  </si>
+  <si>
+    <t>detalhes</t>
+  </si>
+  <si>
+    <t>Descrição principal da ação tomada</t>
+  </si>
+  <si>
+    <t>detalhamento do registro</t>
+  </si>
+  <si>
+    <t>FK_ORDEM_SERVICO_id</t>
+  </si>
+  <si>
+    <t>chave estrangeira de identificação da O.S</t>
+  </si>
+  <si>
+    <t>FK_GRUPO_FUNCIONARIO_id</t>
+  </si>
+  <si>
+    <t>chave estrangeira de indentificação do grupo de funcionário</t>
+  </si>
+  <si>
+    <t>chave estrangeira de indentificação do grupo da O.S</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 82 bytes</t>
+  </si>
+  <si>
+    <t>data da ação realizada</t>
+  </si>
+  <si>
+    <t>dados_os_proposta</t>
+  </si>
+  <si>
+    <t>status_aprovacao</t>
+  </si>
+  <si>
+    <t>PK not nill</t>
+  </si>
+  <si>
+    <t>chave primaria comauto incremento</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>3000 bytes</t>
+  </si>
+  <si>
+    <t>dados da OS proposta (json)</t>
+  </si>
+  <si>
+    <t>status da proposta</t>
+  </si>
+  <si>
+    <t>FK_equipamento_id</t>
+  </si>
+  <si>
+    <t>FK_modelo_ordem_servico_id</t>
+  </si>
+  <si>
+    <t>FK_ocorrencia_id</t>
+  </si>
+  <si>
+    <t>chave estrangeira do equipamento</t>
+  </si>
+  <si>
+    <t>10 byte</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 86 bytes</t>
+  </si>
+  <si>
+    <t>2 byes</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 64 bytes</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 114 bytes</t>
+  </si>
+  <si>
+    <t>modelo</t>
+  </si>
+  <si>
+    <t>chave primaria do modelo da O.S</t>
   </si>
 </sst>
 </file>
@@ -180,7 +514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -451,11 +785,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -515,6 +871,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -545,50 +970,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,15 +1314,15 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="21" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="56.85546875" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" style="21" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="29.5703125" customWidth="1"/>
   </cols>
@@ -950,21 +1333,21 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -978,277 +1361,303 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="36" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="43"/>
+      <c r="B7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="38"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="36" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="34" t="s">
+      <c r="A9" s="42"/>
+      <c r="B9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="37"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="34" t="s">
+      <c r="A10" s="42"/>
+      <c r="B10" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="34" t="s">
+      <c r="A11" s="42"/>
+      <c r="B11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="43"/>
+      <c r="B12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="35"/>
+      <c r="D12" s="38"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="33"/>
+      <c r="D13" s="36" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="36"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="42"/>
+      <c r="D15" s="36" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="41" t="s">
+      <c r="A16" s="42"/>
+      <c r="B16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="42"/>
+      <c r="D16" s="37"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="41" t="s">
+      <c r="A17" s="42"/>
+      <c r="B17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="35"/>
+      <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="41" t="s">
+      <c r="A18" s="42"/>
+      <c r="B18" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="35"/>
+      <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
-      <c r="B19" s="41" t="s">
+      <c r="A19" s="43"/>
+      <c r="B19" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="35"/>
+      <c r="D19" s="38"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="33"/>
+      <c r="D20" s="36" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="36"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="35"/>
+      <c r="D22" s="36" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="41" t="s">
+      <c r="A23" s="39"/>
+      <c r="B23" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="35"/>
+      <c r="D23" s="38"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="35"/>
+      <c r="D24" s="23" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="35"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="36" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="41" t="s">
+      <c r="A26" s="37"/>
+      <c r="B26" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="35"/>
+      <c r="D26" s="37"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="34" t="s">
+      <c r="A27" s="37"/>
+      <c r="B27" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="35"/>
+      <c r="D27" s="37"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="34" t="s">
+      <c r="A28" s="38"/>
+      <c r="B28" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="45"/>
+      <c r="D28" s="38"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="40" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="42"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="40"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="35"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="35"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="43"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="35"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="21">
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="D15:D19"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="B13:B14"/>
@@ -1260,24 +1669,20 @@
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D25:D28"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AD5D63-DE72-4DA9-8FB6-ADFBA61B1A7F}">
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,20 +1696,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1324,14 +1729,26 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="19" t="s">
+        <v>141</v>
+      </c>
       <c r="B7" s="10"/>
       <c r="C7" s="4"/>
       <c r="D7" s="12"/>
@@ -1379,12 +1796,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2661BBEF-BD9B-4A8C-8432-8D2206564E70}">
-  <dimension ref="A2:E14"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,20 +1815,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1431,52 +1848,378 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2661BBEF-BD9B-4A8C-8432-8D2206564E70}">
+  <dimension ref="A2:E16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1491,7 +2234,154 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE60020-624B-4BDA-ADDE-27A9BE674302}">
+  <dimension ref="A2:E14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,20 +2395,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1538,32 +2428,72 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
@@ -1581,7 +2511,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="B14" s="18"/>
     </row>
@@ -1593,12 +2523,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE60020-624B-4BDA-ADDE-27A9BE674302}">
-  <dimension ref="A2:E14"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76EA963-2C1D-4687-9999-1631C8AB029C}">
+  <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,20 +2542,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1645,52 +2575,119 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="18"/>
+      <c r="A9" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1700,12 +2697,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76EA963-2C1D-4687-9999-1631C8AB029C}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C810738D-FFB8-4002-B690-DDD9DD0099E6}">
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,20 +2716,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1752,25 +2749,359 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D1B43B-219C-42AB-BE10-211BABFEA47E}">
+  <dimension ref="A2:E14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FCFBC6-0858-4A1B-A759-12C96CA85BF8}">
+  <dimension ref="A2:E14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>

</xml_diff>

<commit_message>
Atulização do dicionario e dos dados do modelo logico
</commit_message>
<xml_diff>
--- a/db/Dicionário_dados.xlsx
+++ b/db/Dicionário_dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\4DSN_val\BD_conceitual_repairIQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\4DSN_val\BD_repairIQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D65CA2-6DBB-4EE7-9BFA-2145262DB27A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ABE3B0-C817-4C62-B76F-7CF4A6CEA5DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relacionamento" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="152">
   <si>
     <t>Relacionamento</t>
   </si>
@@ -61,9 +61,6 @@
     <t xml:space="preserve">Restrições </t>
   </si>
   <si>
-    <t>Total de bytes da tabela:</t>
-  </si>
-  <si>
     <t>EQUIPAMENTO</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>30 bytes</t>
   </si>
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>10 bytes</t>
   </si>
   <si>
@@ -397,9 +391,6 @@
     <t>chave estrangeira de indentificação do grupo da O.S</t>
   </si>
   <si>
-    <t>Total de bytes da tabela: 82 bytes</t>
-  </si>
-  <si>
     <t>data da ação realizada</t>
   </si>
   <si>
@@ -409,9 +400,6 @@
     <t>status_aprovacao</t>
   </si>
   <si>
-    <t>PK not nill</t>
-  </si>
-  <si>
     <t>chave primaria comauto incremento</t>
   </si>
   <si>
@@ -451,13 +439,52 @@
     <t>Total de bytes da tabela: 64 bytes</t>
   </si>
   <si>
-    <t>Total de bytes da tabela: 114 bytes</t>
-  </si>
-  <si>
     <t>modelo</t>
   </si>
   <si>
     <t>chave primaria do modelo da O.S</t>
+  </si>
+  <si>
+    <t>define o modelo da O.S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 3004 bytes</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela:3006 bytes</t>
+  </si>
+  <si>
+    <t>FK_grupo_funcionario_id</t>
+  </si>
+  <si>
+    <t>FK_ordem_servico_id</t>
+  </si>
+  <si>
+    <t>chave estrangeira de grupo dos funcionarios</t>
+  </si>
+  <si>
+    <t>chave estrangeira de ordem de serviços</t>
+  </si>
+  <si>
+    <t>FK_funcionario_id</t>
+  </si>
+  <si>
+    <t>chave estrangeira de funcionarios</t>
+  </si>
+  <si>
+    <t>FK_equipamentos_id</t>
+  </si>
+  <si>
+    <t>chave estrangeira de equipamentos</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 124 bytes</t>
+  </si>
+  <si>
+    <t>Total de bytes da tabela: 102 bytes</t>
   </si>
 </sst>
 </file>
@@ -916,42 +943,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -969,9 +999,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1313,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,18 +1360,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
@@ -1362,279 +1389,281 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="C6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
+      <c r="B7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="23" t="s">
+      <c r="C7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+      <c r="B9" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="46"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="37"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="23" t="s">
+      <c r="C10" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="46"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="43"/>
+      <c r="B11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C11" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="37"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="23" t="s">
+      <c r="D11" s="46"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="42"/>
+      <c r="B12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="37"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="23" t="s">
-        <v>18</v>
-      </c>
       <c r="C12" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="38"/>
+        <v>13</v>
+      </c>
+      <c r="D12" s="45"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="46"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
+      <c r="B17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="37"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="25" t="s">
+      <c r="D17" s="46"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
+      <c r="B18" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C18" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
-      <c r="B18" s="25" t="s">
+      <c r="D18" s="46"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="42"/>
+      <c r="B19" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="38"/>
+      <c r="D19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="44" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
+      <c r="B23" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="45"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
-        <v>13</v>
+      <c r="A25" s="44" t="s">
+        <v>12</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="23"/>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="46"/>
+      <c r="B26" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="46"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="46"/>
+      <c r="B27" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="46"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="45"/>
+      <c r="B28" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="45"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="37"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="37"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="38"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="25"/>
       <c r="C30" s="23"/>
-      <c r="D30" s="40"/>
+      <c r="D30" s="48"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
       <c r="B31" s="25"/>
       <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
+      <c r="D31" s="23" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
@@ -1650,13 +1679,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D12"/>
     <mergeCell ref="D15:D19"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="D29:D30"/>
@@ -1671,6 +1693,13 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D25:D28"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1681,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AD5D63-DE72-4DA9-8FB6-ADFBA61B1A7F}">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,20 +1725,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1730,29 +1759,37 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="11"/>
+        <v>136</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
@@ -1784,7 +1821,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="B14" s="18"/>
     </row>
@@ -1801,7 +1838,7 @@
   <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,20 +1852,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1849,142 +1886,142 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="E12" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="28"/>
       <c r="C14" s="29"/>
       <c r="D14" s="30"/>
@@ -1992,7 +2029,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="18"/>
     </row>
@@ -2023,20 +2060,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2057,155 +2094,155 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="E10" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>72</v>
-      </c>
       <c r="D11" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>136</v>
-      </c>
       <c r="D14" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2217,7 +2254,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B16" s="18"/>
     </row>
@@ -2248,20 +2285,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2282,70 +2319,70 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="E8" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2364,7 +2401,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14" s="18"/>
     </row>
@@ -2381,7 +2418,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,20 +2432,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2429,70 +2466,70 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2511,7 +2548,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" s="18"/>
     </row>
@@ -2525,6 +2562,180 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76EA963-2C1D-4687-9999-1631C8AB029C}">
+  <dimension ref="A2:E15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C810738D-FFB8-4002-B690-DDD9DD0099E6}">
   <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2542,20 +2753,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2576,116 +2787,126 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="B15" s="18"/>
     </row>
@@ -2697,12 +2918,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C810738D-FFB8-4002-B690-DDD9DD0099E6}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D1B43B-219C-42AB-BE10-211BABFEA47E}">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2716,20 +2937,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2750,87 +2971,87 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2842,7 +3063,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B14" s="18"/>
     </row>
@@ -2854,12 +3075,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D1B43B-219C-42AB-BE10-211BABFEA47E}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FCFBC6-0858-4A1B-A759-12C96CA85BF8}">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,20 +3094,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2907,70 +3128,70 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>116</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2989,144 +3210,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="18"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:E4"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FCFBC6-0858-4A1B-A759-12C96CA85BF8}">
-  <dimension ref="A2:E14"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="B14" s="18"/>
     </row>

</xml_diff>

<commit_message>
Revisão nos documentos do banco de dados e criação do OcorrenciaAdapter
</commit_message>
<xml_diff>
--- a/db/Dicionário_dados.xlsx
+++ b/db/Dicionário_dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\4DSN_val\BD_repairIQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DESENVOLVIMENTO\WORKSYNC\RepairIQ\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ABE3B0-C817-4C62-B76F-7CF4A6CEA5DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C907F4-4B90-496D-BBA7-1EEEB2738CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="2520" windowWidth="21600" windowHeight="11205" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relacionamento" sheetId="4" r:id="rId1"/>
@@ -23,13 +23,27 @@
     <sheet name="REGISTRO AUDITORIA" sheetId="19" r:id="rId8"/>
     <sheet name="PREDITIVA IA" sheetId="20" r:id="rId9"/>
     <sheet name="MODELO ORDEM SERVICO" sheetId="21" r:id="rId10"/>
+    <sheet name="Planilha1" sheetId="22" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="152">
   <si>
     <t>Relacionamento</t>
   </si>
@@ -484,7 +498,7 @@
     <t>Total de bytes da tabela: 124 bytes</t>
   </si>
   <si>
-    <t>Total de bytes da tabela: 102 bytes</t>
+    <t>Total de bytes da tabela:</t>
   </si>
 </sst>
 </file>
@@ -838,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -867,7 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -879,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -891,7 +905,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -916,22 +929,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -943,43 +956,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1018,9 +1028,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1058,9 +1068,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1093,26 +1103,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1145,26 +1138,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1347,9 +1323,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="20" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="56.85546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" style="20" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="29.5703125" customWidth="1"/>
   </cols>
@@ -1360,21 +1336,21 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1388,297 +1364,304 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="35" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="42"/>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="45"/>
+      <c r="D7" s="37"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="35" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="41"/>
+      <c r="B9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="46"/>
+      <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="23" t="s">
+      <c r="A10" s="41"/>
+      <c r="B10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="46"/>
+      <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="45"/>
+      <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="35" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="25" t="s">
+      <c r="A16" s="41"/>
+      <c r="B16" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="46"/>
+      <c r="D16" s="36"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="25" t="s">
+      <c r="A17" s="41"/>
+      <c r="B17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="46"/>
+      <c r="D17" s="36"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="25" t="s">
+      <c r="A18" s="41"/>
+      <c r="B18" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="46"/>
+      <c r="D18" s="36"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="42"/>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="45"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="35" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="42"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="47" t="s">
+      <c r="A22" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="35" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="25" t="s">
+      <c r="A23" s="38"/>
+      <c r="B23" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="45"/>
+      <c r="D23" s="37"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="44" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="35" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="25" t="s">
+      <c r="A26" s="36"/>
+      <c r="B26" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="46"/>
+      <c r="D26" s="36"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="23" t="s">
+      <c r="A27" s="36"/>
+      <c r="B27" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="46"/>
+      <c r="D27" s="36"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
-      <c r="B28" s="23" t="s">
+      <c r="A28" s="37"/>
+      <c r="B28" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="45"/>
+      <c r="D28" s="37"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D29" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="48"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="39"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23" t="s">
+      <c r="A31" s="25"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D12"/>
     <mergeCell ref="D15:D19"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="D29:D30"/>
@@ -1693,13 +1676,6 @@
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D25:D28"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1725,20 +1701,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1775,7 +1751,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>136</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1792,21 +1768,21 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="10"/>
       <c r="C8" s="4"/>
       <c r="D8" s="12"/>
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="10"/>
       <c r="C9" s="4"/>
       <c r="D9" s="12"/>
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="10"/>
       <c r="C10" s="4"/>
       <c r="D10" s="12"/>
@@ -1823,12 +1799,25 @@
       <c r="A14" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:E4"/>
   </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786B41AD-9BC4-411F-94BB-9A3C0633C309}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1852,20 +1841,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1902,7 +1891,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1919,7 +1908,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1936,7 +1925,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1953,7 +1942,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -1987,12 +1976,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="B12" s="10"/>
       <c r="C12" s="4" t="s">
         <v>56</v>
       </c>
@@ -2004,7 +1991,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -2021,17 +2008,16 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2060,20 +2046,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2110,7 +2096,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -2127,7 +2113,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2144,7 +2130,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>67</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -2161,7 +2147,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -2195,7 +2181,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>130</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -2246,17 +2232,16 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2271,7 +2256,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,20 +2270,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2335,11 +2320,11 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>68</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>70</v>
@@ -2352,7 +2337,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2369,7 +2354,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>79</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -2386,7 +2371,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="10"/>
       <c r="C10" s="4"/>
       <c r="D10" s="12"/>
@@ -2403,7 +2388,6 @@
       <c r="A14" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2418,7 +2402,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,20 +2416,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2482,7 +2466,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>84</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -2499,7 +2483,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>87</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2516,7 +2500,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>85</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -2533,7 +2517,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="10"/>
       <c r="C10" s="4"/>
       <c r="D10" s="12"/>
@@ -2550,7 +2534,6 @@
       <c r="A14" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2565,7 +2548,7 @@
   <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,20 +2562,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2618,8 +2601,8 @@
       <c r="B6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>95</v>
+      <c r="C6" s="4">
+        <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>57</v>
@@ -2629,14 +2612,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>92</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>54</v>
+      <c r="C7" s="4">
+        <v>30</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>58</v>
@@ -2646,14 +2629,14 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>93</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>52</v>
+      <c r="C8" s="4">
+        <v>3000</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>58</v>
@@ -2663,14 +2646,14 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>70</v>
+      <c r="C9" s="4">
+        <v>20</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>58</v>
@@ -2680,14 +2663,14 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>117</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>95</v>
+      <c r="C10" s="4">
+        <v>4</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>58</v>
@@ -2697,19 +2680,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="34" t="s">
+      <c r="C11" s="32">
+        <v>4</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="34" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2724,7 +2707,10 @@
       <c r="A15" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15">
+        <f>SUM(C6:C11)</f>
+        <v>3062</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2753,20 +2739,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2803,7 +2789,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>102</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -2820,7 +2806,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2837,7 +2823,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>104</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -2854,7 +2840,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -2871,19 +2857,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="34" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2908,7 +2894,6 @@
       <c r="A15" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2937,20 +2922,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2987,7 +2972,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>110</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -3004,7 +2989,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -3021,7 +3006,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>112</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -3038,7 +3023,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>146</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -3065,7 +3050,6 @@
       <c r="A14" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3094,20 +3078,20 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -3144,7 +3128,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>121</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -3161,7 +3145,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>122</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -3178,7 +3162,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>148</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -3195,7 +3179,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="10"/>
       <c r="C10" s="4"/>
       <c r="D10" s="12"/>
@@ -3212,7 +3196,6 @@
       <c r="A14" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>